<commit_message>
Read write Excel and Json file
</commit_message>
<xml_diff>
--- a/Deepesh/PythonFileHandling/EXCEL_FILE/read_excel_data.xlsx
+++ b/Deepesh/PythonFileHandling/EXCEL_FILE/read_excel_data.xlsx
@@ -2,15 +2,64 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
-  <workbookProtection/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-38520" yWindow="-120" windowWidth="37455" windowHeight="16440" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="Sheet21" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="Sheet22" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet name="Sheet23" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet name="Sheet24" sheetId="6" state="visible" r:id="rId6"/>
+    <sheet name="Sheet25" sheetId="7" state="visible" r:id="rId7"/>
+    <sheet name="Sheet26" sheetId="8" state="visible" r:id="rId8"/>
+    <sheet name="Sheet27" sheetId="9" state="visible" r:id="rId9"/>
+    <sheet name="Sheet28" sheetId="10" state="visible" r:id="rId10"/>
+    <sheet name="Sheet29" sheetId="11" state="visible" r:id="rId11"/>
+    <sheet name="Sheet210" sheetId="12" state="visible" r:id="rId12"/>
+    <sheet name="Sheet211" sheetId="13" state="visible" r:id="rId13"/>
+    <sheet name="Sheet212" sheetId="14" state="visible" r:id="rId14"/>
+    <sheet name="Sheet213" sheetId="15" state="visible" r:id="rId15"/>
+    <sheet name="Sheet214" sheetId="16" state="visible" r:id="rId16"/>
+    <sheet name="Sheet215" sheetId="17" state="visible" r:id="rId17"/>
+    <sheet name="Sheet216" sheetId="18" state="visible" r:id="rId18"/>
+    <sheet name="Sheet217" sheetId="19" state="visible" r:id="rId19"/>
+    <sheet name="Sheet218" sheetId="20" state="visible" r:id="rId20"/>
+    <sheet name="Sheet219" sheetId="21" state="visible" r:id="rId21"/>
+    <sheet name="Sheet220" sheetId="22" state="visible" r:id="rId22"/>
+    <sheet name="Sheet221" sheetId="23" state="visible" r:id="rId23"/>
+    <sheet name="Sheet222" sheetId="24" state="visible" r:id="rId24"/>
+    <sheet name="Sheet223" sheetId="25" state="visible" r:id="rId25"/>
+    <sheet name="Sheet224" sheetId="26" state="visible" r:id="rId26"/>
+    <sheet name="Sheet225" sheetId="27" state="visible" r:id="rId27"/>
+    <sheet name="Sheet226" sheetId="28" state="visible" r:id="rId28"/>
+    <sheet name="Sheet227" sheetId="29" state="visible" r:id="rId29"/>
+    <sheet name="Sheet228" sheetId="30" state="visible" r:id="rId30"/>
+    <sheet name="Sheet229" sheetId="31" state="visible" r:id="rId31"/>
+    <sheet name="Sheet230" sheetId="32" state="visible" r:id="rId32"/>
+    <sheet name="Sheet231" sheetId="33" state="visible" r:id="rId33"/>
+    <sheet name="Sheet232" sheetId="34" state="visible" r:id="rId34"/>
+    <sheet name="Sheet233" sheetId="35" state="visible" r:id="rId35"/>
+    <sheet name="Sheet234" sheetId="36" state="visible" r:id="rId36"/>
+    <sheet name="Sheet235" sheetId="37" state="visible" r:id="rId37"/>
+    <sheet name="Sheet236" sheetId="38" state="visible" r:id="rId38"/>
+    <sheet name="Sheet237" sheetId="39" state="visible" r:id="rId39"/>
+    <sheet name="Sheet238" sheetId="40" state="visible" r:id="rId40"/>
+    <sheet name="Sheet239" sheetId="41" state="visible" r:id="rId41"/>
+    <sheet name="Sheet240" sheetId="42" state="visible" r:id="rId42"/>
+    <sheet name="Sheet241" sheetId="43" state="visible" r:id="rId43"/>
+    <sheet name="Sheet242" sheetId="44" state="visible" r:id="rId44"/>
+    <sheet name="Sheet243" sheetId="45" state="visible" r:id="rId45"/>
+    <sheet name="Sheet244" sheetId="46" state="visible" r:id="rId46"/>
+    <sheet name="Sheet245" sheetId="47" state="visible" r:id="rId47"/>
+    <sheet name="Sheet246" sheetId="48" state="visible" r:id="rId48"/>
+    <sheet name="Sheet247" sheetId="49" state="visible" r:id="rId49"/>
+    <sheet name="Sheet248" sheetId="50" state="visible" r:id="rId50"/>
+    <sheet name="Sheet249" sheetId="51" state="visible" r:id="rId51"/>
   </sheets>
   <definedNames/>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="0" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
@@ -50,7 +99,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
@@ -413,13 +462,13 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <dimension ref="A1:A5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4"/>
   <sheetData>
     <row r="1">
       <c r="A1" t="inlineStr">
@@ -428,6 +477,1390 @@
         </is>
       </c>
     </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Rahul</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Manish</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Pooja</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Mohit</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A8:A8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>535542</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A9:A9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>535543</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A10:A10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>535544</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A11:A11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>535545</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A12:A12"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>535546</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A13:A13"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>535547</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A14:A14"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>535548</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A15:A15"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>535549</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A16:A16"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>535550</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A17:A17"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>535551</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:A9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>535535</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>535536</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>535537</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>535538</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>535539</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>535540</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>535541</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>535542</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>535543</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A18:A18"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>535552</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A19:A19"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>535553</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A20:A20"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>535554</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A21:A21"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>535555</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A22:A22"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>535556</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A23:A23"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>535557</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A24:A24"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>535558</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A25:A25"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>535559</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A26:A26"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>535560</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A27:A27"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>535561</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>535535</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet30.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A28:A28"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>535562</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A29:A29"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>535563</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A30:A30"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>535564</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet33.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A31:A31"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>535565</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet34.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A32:A32"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>535566</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet35.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A33:A33"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>535567</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet36.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A34:A34"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>535568</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet37.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A35:A35"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>535569</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet38.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A36:A36"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>535570</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet39.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A37:A37"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>535571</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A2:A2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>535536</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet40.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A38:A38"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>535572</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet41.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A39:A39"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>535573</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet42.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A40:A40"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>535574</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet43.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A41:A41"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>535575</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet44.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A42:A42"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="42">
+      <c r="A42" t="inlineStr">
+        <is>
+          <t>535576</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet45.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A43:A43"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="43">
+      <c r="A43" t="inlineStr">
+        <is>
+          <t>535577</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet46.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A44:A44"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="44">
+      <c r="A44" t="inlineStr">
+        <is>
+          <t>535578</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet47.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A45:A45"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="45">
+      <c r="A45" t="inlineStr">
+        <is>
+          <t>535579</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet48.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A46:A46"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="46">
+      <c r="A46" t="inlineStr">
+        <is>
+          <t>535580</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet49.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A47:A47"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="47">
+      <c r="A47" t="inlineStr">
+        <is>
+          <t>535581</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A3:A3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>535537</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet50.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A48:A48"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="48">
+      <c r="A48" t="inlineStr">
+        <is>
+          <t>535582</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet51.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A49:A49"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="49">
+      <c r="A49" t="inlineStr">
+        <is>
+          <t>535583</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A4:A4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>535538</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A5:A5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>535539</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A6:A6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>535540</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A7:A7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>535541</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>